<commit_message>
Debugged MLP with max return for long trajectories
</commit_message>
<xml_diff>
--- a/experiments/pg/return_discount_increment/mlp_3x182_no_max_prefix_time_no_clip_grad_step_3e_4_norm_time/oracle_buffer.xlsx
+++ b/experiments/pg/return_discount_increment/mlp_3x182_no_max_prefix_time_no_clip_grad_step_3e_4_norm_time/oracle_buffer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2937"/>
+  <dimension ref="A1:C2938"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38613,6 +38613,19 @@
         <v>14.05723684903867</v>
       </c>
     </row>
+    <row r="2938">
+      <c r="A2938" s="1" t="n">
+        <v>2936</v>
+      </c>
+      <c r="B2938" t="inlineStr">
+        <is>
+          <t>[5, -2, -7]</t>
+        </is>
+      </c>
+      <c r="C2938" t="n">
+        <v>13.98585790195594</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>